<commit_message>
Refactored test specs and added Excel write logic
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="CustomerData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet sheetId="1" name="CustomerData" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Sheet2" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Sheet3" state="visible" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>FirstName</t>
   </si>
@@ -33,6 +33,9 @@
     <t>Mobile</t>
   </si>
   <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
     <t>Gopal</t>
   </si>
   <si>
@@ -45,6 +48,9 @@
     <t>123 Main St</t>
   </si>
   <si>
+    <t>820600</t>
+  </si>
+  <si>
     <t>Ravi</t>
   </si>
   <si>
@@ -57,79 +63,97 @@
     <t>456 Elm Rd</t>
   </si>
   <si>
+    <t>347844</t>
+  </si>
+  <si>
     <t>Bala</t>
   </si>
   <si>
+    <t>TRT</t>
+  </si>
+  <si>
+    <t>TF@gmail.com</t>
+  </si>
+  <si>
+    <t>srfd street</t>
+  </si>
+  <si>
+    <t>513273</t>
+  </si>
+  <si>
     <t>Suresh</t>
   </si>
   <si>
+    <t>KM@gmail.com</t>
+  </si>
+  <si>
+    <t>rft street</t>
+  </si>
+  <si>
+    <t>877341</t>
+  </si>
+  <si>
     <t>Guna</t>
   </si>
   <si>
+    <t>Sekar</t>
+  </si>
+  <si>
+    <t>se@gmail.com</t>
+  </si>
+  <si>
+    <t>sedstreet</t>
+  </si>
+  <si>
+    <t>921465</t>
+  </si>
+  <si>
     <t>Deepan</t>
   </si>
   <si>
+    <t>Kumar@gmail.com</t>
+  </si>
+  <si>
+    <t>ku street</t>
+  </si>
+  <si>
+    <t>619346</t>
+  </si>
+  <si>
     <t>Dhashwin</t>
   </si>
   <si>
-    <t>TRT</t>
-  </si>
-  <si>
-    <t>Sekar</t>
-  </si>
-  <si>
     <t>Gowthami</t>
   </si>
   <si>
-    <t>TF@gmail.com</t>
-  </si>
-  <si>
-    <t>KM@gmail.com</t>
-  </si>
-  <si>
-    <t>se@gmail.com</t>
-  </si>
-  <si>
-    <t>Kumar@gmail.com</t>
-  </si>
-  <si>
     <t>Gow@gmail.com</t>
   </si>
   <si>
-    <t>rft street</t>
-  </si>
-  <si>
-    <t>sedstreet</t>
-  </si>
-  <si>
-    <t>srfd street</t>
-  </si>
-  <si>
-    <t>ku street</t>
-  </si>
-  <si>
     <t>goen street</t>
+  </si>
+  <si>
+    <t>767256</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -175,15 +199,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -476,22 +504,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,124 +536,148 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
         <v>9876543210</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2">
         <v>9123456780</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2">
         <v>9056768900</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2">
         <v>9056768911</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2">
         <v>9056768922</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2">
         <v>9056768933</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2">
         <v>9056768944</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -641,23 +694,123 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2">
+        <v>9056768900</v>
+      </c>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2">
+        <v>9056768911</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9056768922</v>
+      </c>
+    </row>
+    <row r="4" ht="45" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9056768933</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9056768944</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
09/01/2025 new TC added
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>FirstName</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Mobile</t>
   </si>
   <si>
-    <t>Customer ID</t>
+    <t>Customer_ID</t>
   </si>
   <si>
     <t>Gopal</t>
@@ -48,7 +48,7 @@
     <t>123 Main St</t>
   </si>
   <si>
-    <t>820600</t>
+    <t>349467</t>
   </si>
   <si>
     <t>Ravi</t>
@@ -63,7 +63,7 @@
     <t>456 Elm Rd</t>
   </si>
   <si>
-    <t>347844</t>
+    <t>356300</t>
   </si>
   <si>
     <t>Bala</t>
@@ -78,7 +78,7 @@
     <t>srfd street</t>
   </si>
   <si>
-    <t>513273</t>
+    <t>584014</t>
   </si>
   <si>
     <t>Suresh</t>
@@ -90,7 +90,7 @@
     <t>rft street</t>
   </si>
   <si>
-    <t>877341</t>
+    <t>695146</t>
   </si>
   <si>
     <t>Guna</t>
@@ -105,7 +105,7 @@
     <t>sedstreet</t>
   </si>
   <si>
-    <t>921465</t>
+    <t>969209</t>
   </si>
   <si>
     <t>Deepan</t>
@@ -117,7 +117,7 @@
     <t>ku street</t>
   </si>
   <si>
-    <t>619346</t>
+    <t>253850</t>
   </si>
   <si>
     <t>Dhashwin</t>
@@ -132,7 +132,7 @@
     <t>goen street</t>
   </si>
   <si>
-    <t>767256</t>
+    <t>075026</t>
   </si>
 </sst>
 </file>
@@ -504,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -580,123 +580,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2">
-        <v>9056768900</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2">
-        <v>9056768911</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="2">
-        <v>9056768922</v>
-      </c>
-      <c r="F6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2">
-        <v>9056768933</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="2">
-        <v>9056768944</v>
-      </c>
-      <c r="F8" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
-    <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C8" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
@@ -707,7 +602,7 @@
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" ht="30" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -723,8 +618,11 @@
       <c r="E1" s="2">
         <v>9056768900</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" ht="30" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" ht="30" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -740,8 +638,11 @@
       <c r="E2" s="2">
         <v>9056768911</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" ht="30" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" ht="30" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -757,8 +658,11 @@
       <c r="E3" s="2">
         <v>9056768922</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" ht="45" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" ht="45" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -774,8 +678,11 @@
       <c r="E4" s="2">
         <v>9056768933</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" ht="30" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" ht="30" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -790,6 +697,9 @@
       </c>
       <c r="E5" s="2">
         <v>9056768944</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Playwright tests and integrated Allure reporting
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -48,7 +48,7 @@
     <t>123 Main St</t>
   </si>
   <si>
-    <t>349467</t>
+    <t>018317</t>
   </si>
   <si>
     <t>Ravi</t>
@@ -63,7 +63,7 @@
     <t>456 Elm Rd</t>
   </si>
   <si>
-    <t>356300</t>
+    <t>939093</t>
   </si>
   <si>
     <t>Bala</t>

</xml_diff>